<commit_message>
added phishing and training code and some clean up
</commit_message>
<xml_diff>
--- a/training_phishing/training_phishing_template.xlsx
+++ b/training_phishing/training_phishing_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josht\Work\ita_so_phishing_training\training_phishing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEE7206-0752-47B5-89FA-32E9F7463089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C515F9D-FE79-4955-8EFA-741B81140A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -818,7 +818,7 @@
     <col min="5" max="5" width="14.88671875" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
     <col min="7" max="7" width="27.88671875" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="8" max="8" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -972,7 +972,7 @@
     <col min="5" max="5" width="26.6640625" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
     <col min="7" max="7" width="27.88671875" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="8" max="8" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
made changes from feedback
</commit_message>
<xml_diff>
--- a/training_phishing/training_phishing_template.xlsx
+++ b/training_phishing/training_phishing_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josht\Work\ita_so_phishing_training\training_phishing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C515F9D-FE79-4955-8EFA-741B81140A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19981F86-430B-4F86-A7DF-D30409892122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +130,13 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -357,10 +364,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -386,9 +394,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -900,7 +911,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -908,7 +919,7 @@
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -916,7 +927,7 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -924,7 +935,7 @@
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -932,7 +943,7 @@
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -940,7 +951,7 @@
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -948,7 +959,7 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="20"/>
     </row>
   </sheetData>

</xml_diff>